<commit_message>
table pushやりなおし　with CSS
</commit_message>
<xml_diff>
--- a/reference/Core6ResourcesTable.xlsx
+++ b/reference/Core6ResourcesTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kohe/GitHub/clinical-core/reference/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD9427B9-DEA0-8A49-85DA-3D0CD02C8667}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B51D786B-AA6B-5C43-85F6-F1688F42FC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14120" yWindow="460" windowWidth="34900" windowHeight="20880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3940" yWindow="460" windowWidth="34900" windowHeight="20880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AllergyIntoleranceTable" sheetId="2" r:id="rId1"/>
@@ -6012,7 +6012,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="173">
+  <cellXfs count="171">
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
@@ -6397,6 +6397,120 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="16" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="17" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="33" borderId="40" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="33" borderId="41" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="41" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="42" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="34" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="39" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="38" borderId="39" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="43" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="10" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="11" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="38" borderId="11" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="16" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="17" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="40" borderId="17" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="10" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="11" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="11" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="17" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="34" borderId="11" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="43" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="39" borderId="11" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="39" borderId="17" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="38" borderId="17" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="38" borderId="17" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -6411,126 +6525,6 @@
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="16" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="17" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="33" borderId="40" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="33" borderId="41" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="41" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="33" borderId="42" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="34" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="39" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="38" borderId="39" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="39" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="43" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="10" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="11" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="38" borderId="11" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="16" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="17" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="40" borderId="17" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="10" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="11" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="11" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="17" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="34" borderId="11" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="42" xfId="44" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="43" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="39" borderId="11" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="39" borderId="17" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="38" borderId="17" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="38" borderId="17" xfId="44" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="12" xfId="43" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="14" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" xfId="43" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="45">
@@ -10972,22 +10966,22 @@
       <c r="I72" s="33"/>
     </row>
     <row r="73" spans="1:9" ht="30">
-      <c r="A73" s="132"/>
-      <c r="B73" s="128" t="s">
+      <c r="A73" s="170"/>
+      <c r="B73" s="166" t="s">
         <v>356</v>
       </c>
-      <c r="C73" s="128"/>
-      <c r="D73" s="128"/>
-      <c r="E73" s="128" t="s">
+      <c r="C73" s="166"/>
+      <c r="D73" s="166"/>
+      <c r="E73" s="166" t="s">
         <v>51</v>
       </c>
-      <c r="F73" s="128" t="s">
+      <c r="F73" s="166" t="s">
         <v>52</v>
       </c>
-      <c r="G73" s="128" t="s">
+      <c r="G73" s="166" t="s">
         <v>357</v>
       </c>
-      <c r="H73" s="129" t="s">
+      <c r="H73" s="167" t="s">
         <v>294</v>
       </c>
       <c r="I73" s="33" t="s">
@@ -10995,27 +10989,27 @@
       </c>
     </row>
     <row r="74" spans="1:9">
-      <c r="A74" s="132"/>
-      <c r="B74" s="128"/>
-      <c r="C74" s="128"/>
-      <c r="D74" s="128"/>
-      <c r="E74" s="128"/>
-      <c r="F74" s="128"/>
-      <c r="G74" s="128"/>
-      <c r="H74" s="130"/>
+      <c r="A74" s="170"/>
+      <c r="B74" s="166"/>
+      <c r="C74" s="166"/>
+      <c r="D74" s="166"/>
+      <c r="E74" s="166"/>
+      <c r="F74" s="166"/>
+      <c r="G74" s="166"/>
+      <c r="H74" s="168"/>
       <c r="I74" s="33" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="75" spans="1:9">
-      <c r="A75" s="132"/>
-      <c r="B75" s="128"/>
-      <c r="C75" s="128"/>
-      <c r="D75" s="128"/>
-      <c r="E75" s="128"/>
-      <c r="F75" s="128"/>
-      <c r="G75" s="128"/>
-      <c r="H75" s="131"/>
+      <c r="A75" s="170"/>
+      <c r="B75" s="166"/>
+      <c r="C75" s="166"/>
+      <c r="D75" s="166"/>
+      <c r="E75" s="166"/>
+      <c r="F75" s="166"/>
+      <c r="G75" s="166"/>
+      <c r="H75" s="169"/>
       <c r="I75" s="33" t="s">
         <v>284</v>
       </c>
@@ -11215,8 +11209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDAA13D8-BBCA-8249-9865-5E438A955DB5}">
   <dimension ref="A1:I56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="171" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G37" sqref="G37"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="171" zoomScaleNormal="110" workbookViewId="0">
+      <selection sqref="A1:I56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
@@ -11233,71 +11227,71 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="76" thickBot="1">
-      <c r="A1" s="138" t="s">
+      <c r="A1" s="133" t="s">
         <v>374</v>
       </c>
-      <c r="B1" s="139" t="s">
+      <c r="B1" s="134" t="s">
         <v>375</v>
       </c>
-      <c r="C1" s="139" t="s">
+      <c r="C1" s="134" t="s">
         <v>376</v>
       </c>
-      <c r="D1" s="139" t="s">
+      <c r="D1" s="134" t="s">
         <v>377</v>
       </c>
-      <c r="E1" s="140" t="s">
+      <c r="E1" s="135" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="140" t="s">
+      <c r="F1" s="135" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="140" t="s">
+      <c r="G1" s="135" t="s">
         <v>302</v>
       </c>
-      <c r="H1" s="140" t="s">
+      <c r="H1" s="135" t="s">
         <v>482</v>
       </c>
-      <c r="I1" s="141" t="s">
+      <c r="I1" s="136" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="31" thickBot="1">
-      <c r="A2" s="142" t="s">
+      <c r="A2" s="137" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="143"/>
-      <c r="C2" s="143"/>
-      <c r="D2" s="143"/>
-      <c r="E2" s="144" t="s">
+      <c r="B2" s="138"/>
+      <c r="C2" s="138"/>
+      <c r="D2" s="138"/>
+      <c r="E2" s="139" t="s">
         <v>378</v>
       </c>
-      <c r="F2" s="145"/>
-      <c r="G2" s="145" t="s">
+      <c r="F2" s="140"/>
+      <c r="G2" s="140" t="s">
         <v>367</v>
       </c>
       <c r="H2" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="146" t="s">
+      <c r="I2" s="141" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="147" t="s">
+      <c r="A3" s="142" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="148"/>
-      <c r="C3" s="148"/>
-      <c r="D3" s="148"/>
-      <c r="E3" s="149" t="s">
+      <c r="B3" s="143"/>
+      <c r="C3" s="143"/>
+      <c r="D3" s="143"/>
+      <c r="E3" s="144" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="150" t="s">
+      <c r="F3" s="145" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="150"/>
-      <c r="H3" s="150"/>
-      <c r="I3" s="151"/>
+      <c r="G3" s="145"/>
+      <c r="H3" s="145"/>
+      <c r="I3" s="146"/>
     </row>
     <row r="4" spans="1:9" ht="270">
       <c r="A4" s="49" t="s">
@@ -11398,17 +11392,17 @@
       </c>
     </row>
     <row r="8" spans="1:9" s="54" customFormat="1" ht="31" thickBot="1">
-      <c r="A8" s="152" t="s">
+      <c r="A8" s="147" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="153" t="s">
+      <c r="B8" s="148" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="153" t="s">
+      <c r="C8" s="148" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="153"/>
-      <c r="E8" s="154" t="s">
+      <c r="D8" s="148"/>
+      <c r="E8" s="149" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="91" t="s">
@@ -11420,26 +11414,26 @@
       <c r="H8" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="I8" s="155" t="s">
+      <c r="I8" s="150" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="54" customFormat="1">
-      <c r="A9" s="156" t="s">
+      <c r="A9" s="151" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="157"/>
-      <c r="C9" s="157"/>
-      <c r="D9" s="157"/>
-      <c r="E9" s="158" t="s">
+      <c r="B9" s="152"/>
+      <c r="C9" s="152"/>
+      <c r="D9" s="152"/>
+      <c r="E9" s="153" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="159"/>
-      <c r="G9" s="159" t="s">
+      <c r="F9" s="154"/>
+      <c r="G9" s="154" t="s">
         <v>186</v>
       </c>
-      <c r="H9" s="159"/>
-      <c r="I9" s="160"/>
+      <c r="H9" s="154"/>
+      <c r="I9" s="155"/>
     </row>
     <row r="10" spans="1:9" s="54" customFormat="1" ht="75">
       <c r="A10" s="49" t="s">
@@ -11461,13 +11455,13 @@
       <c r="I10" s="51"/>
     </row>
     <row r="11" spans="1:9" s="54" customFormat="1" ht="136" thickBot="1">
-      <c r="A11" s="152" t="s">
+      <c r="A11" s="147" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="153"/>
-      <c r="C11" s="153"/>
-      <c r="D11" s="153"/>
-      <c r="E11" s="161" t="s">
+      <c r="B11" s="148"/>
+      <c r="C11" s="148"/>
+      <c r="D11" s="148"/>
+      <c r="E11" s="156" t="s">
         <v>43</v>
       </c>
       <c r="F11" s="91" t="s">
@@ -11477,28 +11471,28 @@
         <v>379</v>
       </c>
       <c r="H11" s="91"/>
-      <c r="I11" s="155"/>
+      <c r="I11" s="150"/>
     </row>
     <row r="12" spans="1:9" s="54" customFormat="1" ht="45">
-      <c r="A12" s="156" t="s">
+      <c r="A12" s="151" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="157" t="s">
+      <c r="B12" s="152" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="157"/>
-      <c r="D12" s="157"/>
-      <c r="E12" s="162" t="s">
+      <c r="C12" s="152"/>
+      <c r="D12" s="152"/>
+      <c r="E12" s="157" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="159" t="s">
+      <c r="F12" s="154" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="159"/>
-      <c r="H12" s="159" t="s">
+      <c r="G12" s="154"/>
+      <c r="H12" s="154" t="s">
         <v>11</v>
       </c>
-      <c r="I12" s="163" t="s">
+      <c r="I12" s="158" t="s">
         <v>184</v>
       </c>
     </row>
@@ -11603,92 +11597,92 @@
       </c>
     </row>
     <row r="17" spans="1:9" ht="21" thickBot="1">
-      <c r="A17" s="152" t="s">
+      <c r="A17" s="147" t="s">
         <v>46</v>
       </c>
-      <c r="B17" s="134" t="s">
+      <c r="B17" s="129" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="134"/>
-      <c r="D17" s="134"/>
-      <c r="E17" s="161" t="s">
+      <c r="C17" s="129"/>
+      <c r="D17" s="129"/>
+      <c r="E17" s="156" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="136" t="s">
+      <c r="F17" s="131" t="s">
         <v>48</v>
       </c>
-      <c r="G17" s="136" t="s">
+      <c r="G17" s="131" t="s">
         <v>311</v>
       </c>
       <c r="H17" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="I17" s="137" t="s">
+      <c r="I17" s="132" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="31" thickBot="1">
-      <c r="A18" s="142" t="s">
+      <c r="A18" s="137" t="s">
         <v>306</v>
       </c>
-      <c r="B18" s="143"/>
-      <c r="C18" s="143"/>
-      <c r="D18" s="143"/>
-      <c r="E18" s="144" t="s">
+      <c r="B18" s="138"/>
+      <c r="C18" s="138"/>
+      <c r="D18" s="138"/>
+      <c r="E18" s="139" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="145" t="s">
+      <c r="F18" s="140" t="s">
         <v>31</v>
       </c>
-      <c r="G18" s="145" t="s">
+      <c r="G18" s="140" t="s">
         <v>384</v>
       </c>
       <c r="H18" s="93" t="s">
         <v>11</v>
       </c>
-      <c r="I18" s="164" t="s">
+      <c r="I18" s="159" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="21" thickBot="1">
-      <c r="A19" s="142" t="s">
+      <c r="A19" s="137" t="s">
         <v>313</v>
       </c>
-      <c r="B19" s="143"/>
-      <c r="C19" s="143"/>
-      <c r="D19" s="143"/>
-      <c r="E19" s="144" t="s">
+      <c r="B19" s="138"/>
+      <c r="C19" s="138"/>
+      <c r="D19" s="138"/>
+      <c r="E19" s="139" t="s">
         <v>10</v>
       </c>
-      <c r="F19" s="145" t="s">
+      <c r="F19" s="140" t="s">
         <v>31</v>
       </c>
-      <c r="G19" s="145" t="s">
+      <c r="G19" s="140" t="s">
         <v>385</v>
       </c>
-      <c r="H19" s="145"/>
-      <c r="I19" s="164" t="s">
+      <c r="H19" s="140"/>
+      <c r="I19" s="159" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="32" customHeight="1">
-      <c r="A20" s="147" t="s">
+      <c r="A20" s="142" t="s">
         <v>386</v>
       </c>
-      <c r="B20" s="148"/>
-      <c r="C20" s="148"/>
-      <c r="D20" s="148"/>
-      <c r="E20" s="165" t="s">
+      <c r="B20" s="143"/>
+      <c r="C20" s="143"/>
+      <c r="D20" s="143"/>
+      <c r="E20" s="160" t="s">
         <v>387</v>
       </c>
-      <c r="F20" s="150" t="s">
+      <c r="F20" s="145" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="150" t="s">
+      <c r="G20" s="145" t="s">
         <v>388</v>
       </c>
-      <c r="H20" s="150"/>
-      <c r="I20" s="151"/>
+      <c r="H20" s="145"/>
+      <c r="I20" s="146"/>
     </row>
     <row r="21" spans="1:9" ht="102" customHeight="1">
       <c r="A21" s="44" t="s">
@@ -11741,48 +11735,48 @@
       </c>
     </row>
     <row r="23" spans="1:9" ht="58" customHeight="1" thickBot="1">
-      <c r="A23" s="133" t="s">
+      <c r="A23" s="128" t="s">
         <v>392</v>
       </c>
-      <c r="B23" s="134" t="s">
+      <c r="B23" s="129" t="s">
         <v>396</v>
       </c>
-      <c r="C23" s="134"/>
-      <c r="D23" s="134"/>
-      <c r="E23" s="166" t="s">
+      <c r="C23" s="129"/>
+      <c r="D23" s="129"/>
+      <c r="E23" s="161" t="s">
         <v>387</v>
       </c>
-      <c r="F23" s="136" t="s">
+      <c r="F23" s="131" t="s">
         <v>48</v>
       </c>
-      <c r="G23" s="136" t="s">
+      <c r="G23" s="131" t="s">
         <v>397</v>
       </c>
       <c r="H23" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="I23" s="137" t="s">
+      <c r="I23" s="132" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="45">
-      <c r="A24" s="147" t="s">
+      <c r="A24" s="142" t="s">
         <v>315</v>
       </c>
-      <c r="B24" s="148"/>
-      <c r="C24" s="148"/>
-      <c r="D24" s="148"/>
-      <c r="E24" s="149" t="s">
+      <c r="B24" s="143"/>
+      <c r="C24" s="143"/>
+      <c r="D24" s="143"/>
+      <c r="E24" s="144" t="s">
         <v>378</v>
       </c>
-      <c r="F24" s="150" t="s">
+      <c r="F24" s="145" t="s">
         <v>52</v>
       </c>
-      <c r="G24" s="150" t="s">
+      <c r="G24" s="145" t="s">
         <v>399</v>
       </c>
-      <c r="H24" s="150"/>
-      <c r="I24" s="151"/>
+      <c r="H24" s="145"/>
+      <c r="I24" s="146"/>
     </row>
     <row r="25" spans="1:9" ht="28">
       <c r="A25" s="44" t="s">
@@ -11858,52 +11852,52 @@
       </c>
     </row>
     <row r="28" spans="1:9" ht="31" thickBot="1">
-      <c r="A28" s="133" t="s">
+      <c r="A28" s="128" t="s">
         <v>315</v>
       </c>
-      <c r="B28" s="134" t="s">
+      <c r="B28" s="129" t="s">
         <v>403</v>
       </c>
-      <c r="C28" s="134" t="s">
+      <c r="C28" s="129" t="s">
         <v>153</v>
       </c>
-      <c r="D28" s="134"/>
-      <c r="E28" s="167" t="s">
+      <c r="D28" s="129"/>
+      <c r="E28" s="162" t="s">
         <v>10</v>
       </c>
-      <c r="F28" s="136" t="s">
+      <c r="F28" s="131" t="s">
         <v>48</v>
       </c>
-      <c r="G28" s="136" t="s">
+      <c r="G28" s="131" t="s">
         <v>405</v>
       </c>
       <c r="H28" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="I28" s="137" t="s">
+      <c r="I28" s="132" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="54" customFormat="1" ht="105">
-      <c r="A29" s="156" t="s">
+      <c r="A29" s="151" t="s">
         <v>266</v>
       </c>
-      <c r="B29" s="157"/>
-      <c r="C29" s="157"/>
-      <c r="D29" s="157"/>
-      <c r="E29" s="162" t="s">
+      <c r="B29" s="152"/>
+      <c r="C29" s="152"/>
+      <c r="D29" s="152"/>
+      <c r="E29" s="157" t="s">
         <v>10</v>
       </c>
-      <c r="F29" s="159" t="s">
+      <c r="F29" s="154" t="s">
         <v>82</v>
       </c>
-      <c r="G29" s="159" t="s">
+      <c r="G29" s="154" t="s">
         <v>372</v>
       </c>
-      <c r="H29" s="159" t="s">
+      <c r="H29" s="154" t="s">
         <v>17</v>
       </c>
-      <c r="I29" s="160" t="s">
+      <c r="I29" s="155" t="s">
         <v>263</v>
       </c>
     </row>
@@ -11925,11 +11919,11 @@
       </c>
     </row>
     <row r="31" spans="1:9" s="54" customFormat="1" ht="201" customHeight="1" thickBot="1">
-      <c r="A31" s="152"/>
-      <c r="B31" s="153"/>
-      <c r="C31" s="153"/>
-      <c r="D31" s="153"/>
-      <c r="E31" s="168"/>
+      <c r="A31" s="147"/>
+      <c r="B31" s="148"/>
+      <c r="C31" s="148"/>
+      <c r="D31" s="148"/>
+      <c r="E31" s="163"/>
       <c r="F31" s="91"/>
       <c r="G31" s="91" t="s">
         <v>267</v>
@@ -11937,114 +11931,114 @@
       <c r="H31" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="I31" s="155" t="s">
+      <c r="I31" s="150" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:9" ht="31" thickBot="1">
-      <c r="A32" s="142" t="s">
+      <c r="A32" s="137" t="s">
         <v>319</v>
       </c>
-      <c r="B32" s="143"/>
-      <c r="C32" s="143"/>
-      <c r="D32" s="143"/>
-      <c r="E32" s="144" t="s">
+      <c r="B32" s="138"/>
+      <c r="C32" s="138"/>
+      <c r="D32" s="138"/>
+      <c r="E32" s="139" t="s">
         <v>245</v>
       </c>
-      <c r="F32" s="145" t="s">
+      <c r="F32" s="140" t="s">
         <v>93</v>
       </c>
-      <c r="G32" s="145" t="s">
+      <c r="G32" s="140" t="s">
         <v>406</v>
       </c>
       <c r="H32" s="93" t="s">
         <v>17</v>
       </c>
-      <c r="I32" s="164" t="s">
+      <c r="I32" s="159" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="33" spans="1:9" ht="30">
-      <c r="A33" s="147" t="s">
+      <c r="A33" s="142" t="s">
         <v>407</v>
       </c>
-      <c r="B33" s="148"/>
-      <c r="C33" s="148"/>
-      <c r="D33" s="148"/>
-      <c r="E33" s="169" t="s">
+      <c r="B33" s="143"/>
+      <c r="C33" s="143"/>
+      <c r="D33" s="143"/>
+      <c r="E33" s="164" t="s">
         <v>408</v>
       </c>
-      <c r="F33" s="150" t="s">
+      <c r="F33" s="145" t="s">
         <v>136</v>
       </c>
-      <c r="G33" s="150" t="s">
+      <c r="G33" s="145" t="s">
         <v>409</v>
       </c>
-      <c r="H33" s="150"/>
-      <c r="I33" s="170"/>
+      <c r="H33" s="145"/>
+      <c r="I33" s="165"/>
     </row>
     <row r="34" spans="1:9" ht="61" thickBot="1">
-      <c r="A34" s="133" t="s">
+      <c r="A34" s="128" t="s">
         <v>410</v>
       </c>
-      <c r="B34" s="134" t="s">
+      <c r="B34" s="129" t="s">
         <v>61</v>
       </c>
-      <c r="C34" s="134"/>
-      <c r="D34" s="134"/>
-      <c r="E34" s="135" t="s">
+      <c r="C34" s="129"/>
+      <c r="D34" s="129"/>
+      <c r="E34" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="F34" s="136" t="s">
+      <c r="F34" s="131" t="s">
         <v>145</v>
       </c>
-      <c r="G34" s="136" t="s">
+      <c r="G34" s="131" t="s">
         <v>411</v>
       </c>
       <c r="H34" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="I34" s="137" t="s">
+      <c r="I34" s="132" t="s">
         <v>321</v>
       </c>
     </row>
     <row r="35" spans="1:9" ht="31" thickBot="1">
-      <c r="A35" s="142" t="s">
+      <c r="A35" s="137" t="s">
         <v>412</v>
       </c>
-      <c r="B35" s="143"/>
-      <c r="C35" s="143"/>
-      <c r="D35" s="143"/>
-      <c r="E35" s="144" t="s">
+      <c r="B35" s="138"/>
+      <c r="C35" s="138"/>
+      <c r="D35" s="138"/>
+      <c r="E35" s="139" t="s">
         <v>413</v>
       </c>
-      <c r="F35" s="145" t="s">
+      <c r="F35" s="140" t="s">
         <v>322</v>
       </c>
-      <c r="G35" s="145" t="s">
+      <c r="G35" s="140" t="s">
         <v>480</v>
       </c>
-      <c r="H35" s="145"/>
-      <c r="I35" s="164"/>
+      <c r="H35" s="140"/>
+      <c r="I35" s="159"/>
     </row>
     <row r="36" spans="1:9" ht="30">
-      <c r="A36" s="147" t="s">
+      <c r="A36" s="142" t="s">
         <v>560</v>
       </c>
-      <c r="B36" s="148"/>
-      <c r="C36" s="148"/>
-      <c r="D36" s="148"/>
-      <c r="E36" s="172" t="s">
+      <c r="B36" s="143"/>
+      <c r="C36" s="143"/>
+      <c r="D36" s="143"/>
+      <c r="E36" s="164" t="s">
         <v>243</v>
       </c>
-      <c r="F36" s="150" t="s">
+      <c r="F36" s="145" t="s">
         <v>148</v>
       </c>
-      <c r="G36" s="150" t="s">
+      <c r="G36" s="145" t="s">
         <v>561</v>
       </c>
-      <c r="H36" s="150"/>
-      <c r="I36" s="151"/>
+      <c r="H36" s="145"/>
+      <c r="I36" s="146"/>
     </row>
     <row r="37" spans="1:9" ht="28">
       <c r="A37" s="44" t="s">
@@ -12099,7 +12093,7 @@
         <v>327</v>
       </c>
       <c r="D39" s="45"/>
-      <c r="E39" s="171" t="s">
+      <c r="E39" s="42" t="s">
         <v>10</v>
       </c>
       <c r="F39" s="41" t="s">
@@ -12374,29 +12368,29 @@
       </c>
     </row>
     <row r="50" spans="1:9" ht="29" thickBot="1">
-      <c r="A50" s="133" t="s">
+      <c r="A50" s="128" t="s">
         <v>323</v>
       </c>
-      <c r="B50" s="134" t="s">
+      <c r="B50" s="129" t="s">
         <v>341</v>
       </c>
-      <c r="C50" s="134" t="s">
+      <c r="C50" s="129" t="s">
         <v>31</v>
       </c>
-      <c r="D50" s="134"/>
-      <c r="E50" s="135" t="s">
+      <c r="D50" s="129"/>
+      <c r="E50" s="130" t="s">
         <v>10</v>
       </c>
-      <c r="F50" s="136" t="s">
+      <c r="F50" s="131" t="s">
         <v>31</v>
       </c>
-      <c r="G50" s="136" t="s">
+      <c r="G50" s="131" t="s">
         <v>423</v>
       </c>
       <c r="H50" s="91" t="s">
         <v>418</v>
       </c>
-      <c r="I50" s="137" t="s">
+      <c r="I50" s="132" t="s">
         <v>346</v>
       </c>
     </row>
@@ -12520,31 +12514,31 @@
       </c>
     </row>
     <row r="56" spans="1:9" ht="29" thickBot="1">
-      <c r="A56" s="133" t="s">
+      <c r="A56" s="128" t="s">
         <v>347</v>
       </c>
-      <c r="B56" s="134" t="s">
+      <c r="B56" s="129" t="s">
         <v>348</v>
       </c>
-      <c r="C56" s="134" t="s">
+      <c r="C56" s="129" t="s">
         <v>403</v>
       </c>
-      <c r="D56" s="134" t="s">
+      <c r="D56" s="129" t="s">
         <v>153</v>
       </c>
-      <c r="E56" s="135" t="s">
+      <c r="E56" s="130" t="s">
         <v>51</v>
       </c>
-      <c r="F56" s="136" t="s">
+      <c r="F56" s="131" t="s">
         <v>48</v>
       </c>
-      <c r="G56" s="136" t="s">
+      <c r="G56" s="131" t="s">
         <v>352</v>
       </c>
       <c r="H56" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="I56" s="137" t="s">
+      <c r="I56" s="132" t="s">
         <v>353</v>
       </c>
     </row>

</xml_diff>